<commit_message>
Sales Order Module Creating Feature
</commit_message>
<xml_diff>
--- a/data/CRM.xlsx
+++ b/data/CRM.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CBC2B809-62E3-45DF-A832-35C6BCF28ADA}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="11970" windowHeight="8415" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="11970" windowHeight="8415" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Campaign" sheetId="2" r:id="rId1"/>
     <sheet name="CreateCampaign" sheetId="3" r:id="rId2"/>
+    <sheet name="CreateSO" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:L26"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="88">
   <si>
     <t>ErrorMessage</t>
   </si>
@@ -213,13 +214,85 @@
   </si>
   <si>
     <t>dell1</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>ErrorMsg</t>
+  </si>
+  <si>
+    <t>LoginPageTitle</t>
+  </si>
+  <si>
+    <t>HomePageTitle</t>
+  </si>
+  <si>
+    <t>SalesOrderPage</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>CustomerNumber</t>
+  </si>
+  <si>
+    <t>CarrierName</t>
+  </si>
+  <si>
+    <t>Salescommision</t>
+  </si>
+  <si>
+    <t>Due Date</t>
+  </si>
+  <si>
+    <t>ad123</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>No such account configured for the user</t>
+  </si>
+  <si>
+    <t>Zoho CRM - Home Page</t>
+  </si>
+  <si>
+    <t>Hp laptop</t>
+  </si>
+  <si>
+    <t>007</t>
+  </si>
+  <si>
+    <t>BlueDart</t>
+  </si>
+  <si>
+    <t>11/27/2019</t>
+  </si>
+  <si>
+    <t>ad min</t>
+  </si>
+  <si>
+    <t>ad$^%&amp;</t>
+  </si>
+  <si>
+    <t>ad123%^&amp;</t>
+  </si>
+  <si>
+    <t>123456</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,6 +310,13 @@
     <font>
       <b/>
       <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -269,11 +349,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -546,251 +629,251 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A46"/>
   <sheetViews>
     <sheetView topLeftCell="A32" workbookViewId="0">
       <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="18.75">
+    <row r="1" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="18.75">
+    <row r="3" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="18.75">
+    <row r="5" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="18.75">
+    <row r="7" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="18.75">
+    <row r="9" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="18.75">
+    <row r="11" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="18.75">
+    <row r="13" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="18.75">
+    <row r="15" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="18.75">
+    <row r="17" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="18.75">
+    <row r="19" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="18.75">
+    <row r="21" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="18.75">
+    <row r="23" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="18.75">
+    <row r="25" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:1" ht="18.75">
+    <row r="27" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:1" ht="18.75">
+    <row r="29" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:1" ht="18.75">
+    <row r="31" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="18.75">
+    <row r="33" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="18.75">
+    <row r="35" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:1" ht="18.75">
+    <row r="37" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="1:1" ht="18.75">
+    <row r="39" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="18.75">
+    <row r="41" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:1" ht="18.75">
+    <row r="43" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="45" spans="1:1" ht="18.75">
+    <row r="45" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>40</v>
       </c>
@@ -801,16 +884,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AX3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:50" ht="21">
+    <row r="1" spans="1:50" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>41</v>
       </c>
@@ -890,7 +973,7 @@
       <c r="AW1" s="2"/>
       <c r="AX1" s="2"/>
     </row>
-    <row r="2" spans="1:50">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>55</v>
       </c>
@@ -970,10 +1053,207 @@
       <c r="AW2" s="3"/>
       <c r="AX2" s="3"/>
     </row>
-    <row r="3" spans="1:50">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>63</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A66A832-6AF9-4E2C-AA71-E3F18211CD67}">
+  <dimension ref="A1:M7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:M7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="3">
+        <v>123456</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="K2" s="3">
+        <v>1000</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="3">
+        <v>123456</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="3">
+        <v>123456</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>12345</v>
+      </c>
+      <c r="B6" s="3">
+        <v>123456</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>45678</v>
+      </c>
+      <c r="B7" s="3">
+        <v>123456</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
changed the BaseTest Code
</commit_message>
<xml_diff>
--- a/data/CRM.xlsx
+++ b/data/CRM.xlsx
@@ -1,14 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CBC2B809-62E3-45DF-A832-35C6BCF28ADA}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="11970" windowHeight="8415" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="11970" windowHeight="8415"/>
   </bookViews>
   <sheets>
-    <sheet name="Campaign" sheetId="2" r:id="rId1"/>
+    <sheet name="Contacts" sheetId="2" r:id="rId1"/>
     <sheet name="CreateCampaign" sheetId="3" r:id="rId2"/>
     <sheet name="CreateSO" sheetId="4" r:id="rId3"/>
   </sheets>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="93">
   <si>
     <t>ErrorMessage</t>
   </si>
@@ -39,9 +38,6 @@
     <t>Login Page</t>
   </si>
   <si>
-    <t>Tasks List</t>
-  </si>
-  <si>
     <t>Campaign Page</t>
   </si>
   <si>
@@ -286,12 +282,30 @@
   </si>
   <si>
     <t>123456</t>
+  </si>
+  <si>
+    <t>Contact LN</t>
+  </si>
+  <si>
+    <t>Biradar</t>
+  </si>
+  <si>
+    <t>Maialing Street</t>
+  </si>
+  <si>
+    <t>JP Nagar</t>
+  </si>
+  <si>
+    <t>http://192.168.150.128:8080/crm/ShowHomePage.do</t>
+  </si>
+  <si>
+    <t>url1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -636,255 +650,277 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="6" max="6" width="54" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="13" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+    <row r="15" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="39" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="41" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AX3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -895,46 +931,46 @@
   <sheetData>
     <row r="1" spans="1:50" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
@@ -975,10 +1011,10 @@
     </row>
     <row r="2" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="C2" s="3">
         <v>120000</v>
@@ -987,34 +1023,34 @@
         <v>400000</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>58</v>
       </c>
       <c r="G2" s="3">
         <v>500000</v>
       </c>
       <c r="H2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="M2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>12</v>
       </c>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
@@ -1055,7 +1091,7 @@
     </row>
     <row r="3" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1064,10 +1100,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A66A832-6AF9-4E2C-AA71-E3F18211CD67}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:M7"/>
     </sheetView>
   </sheetViews>
@@ -1075,95 +1111,95 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B2" s="3">
         <v>123456</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>77</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>78</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>82</v>
       </c>
       <c r="K2" s="3">
         <v>1000</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3" s="3">
         <v>123456</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -1177,13 +1213,13 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B4" s="3">
         <v>123456</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -1197,13 +1233,13 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>87</v>
-      </c>
       <c r="C5" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -1223,7 +1259,7 @@
         <v>123456</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -1243,7 +1279,7 @@
         <v>123456</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>

</xml_diff>

<commit_message>
Create Potential Excel File
</commit_message>
<xml_diff>
--- a/data/CRM.xlsx
+++ b/data/CRM.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEA00F27-E042-4D95-BE43-42243DB49589}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Contacts" sheetId="2" r:id="rId1"/>
     <sheet name="CloneContact" sheetId="5" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId3"/>
+    <sheet name="createpotential" sheetId="6" r:id="rId3"/>
     <sheet name="CreateCampaign" sheetId="3" r:id="rId4"/>
     <sheet name="CreateSO" sheetId="4" r:id="rId5"/>
     <sheet name="CRMCampaign" sheetId="7" r:id="rId6"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="111">
   <si>
     <t>ErrorMessage</t>
   </si>
@@ -335,12 +334,36 @@
   </si>
   <si>
     <t>Clone Campaign</t>
+  </si>
+  <si>
+    <t>Login tilte</t>
+  </si>
+  <si>
+    <t>Hometitle</t>
+  </si>
+  <si>
+    <t>Potential page</t>
+  </si>
+  <si>
+    <t>NewPotential</t>
+  </si>
+  <si>
+    <t>Potential name</t>
+  </si>
+  <si>
+    <t>ClosingDate</t>
+  </si>
+  <si>
+    <t>jack</t>
+  </si>
+  <si>
+    <t>11/30/2019</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -702,22 +725,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.109375" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
     <col min="6" max="6" width="54" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -731,7 +754,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -745,222 +768,222 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="45" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>39</v>
       </c>
@@ -972,16 +995,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>93</v>
       </c>
@@ -995,7 +1018,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1015,28 +1038,71 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7F8C912-CFD4-4283-8CAD-047CC438A622}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AX3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:50" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:50" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>40</v>
       </c>
@@ -1116,7 +1182,7 @@
       <c r="AW1" s="2"/>
       <c r="AX1" s="2"/>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>54</v>
       </c>
@@ -1196,7 +1262,7 @@
       <c r="AW2" s="3"/>
       <c r="AX2" s="3"/>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>62</v>
       </c>
@@ -1207,16 +1273,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>63</v>
       </c>
@@ -1257,7 +1323,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>75</v>
       </c>
@@ -1298,7 +1364,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>83</v>
       </c>
@@ -1318,7 +1384,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>84</v>
       </c>
@@ -1338,7 +1404,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>85</v>
       </c>
@@ -1358,7 +1424,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>12345</v>
       </c>
@@ -1378,7 +1444,7 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>45678</v>
       </c>
@@ -1404,16 +1470,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B98438F-69BA-47C2-AF38-C52F0F1A8CFC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>98</v>
       </c>
@@ -1430,7 +1496,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1453,12 +1519,12 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D129A4-0F5C-416A-877D-A29583829E89}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>